<commit_message>
Added a new field in the report as End User Accepted
</commit_message>
<xml_diff>
--- a/data/input/compare/mapping/Mapping.xlsx
+++ b/data/input/compare/mapping/Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Back-Ups\ExcelReportAnalyzer\xlreportanalyzer\data\input\compare\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B966BD-3232-42C5-A46C-A7FBDD759B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B28BA2-93B7-484F-8FBD-53AFC1E05F19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="1284" windowWidth="20364" windowHeight="11076" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="217">
   <si>
     <t>PORTFOLIO_CODE</t>
   </si>
@@ -682,6 +682,12 @@
   </si>
   <si>
     <t>Tolerance(10)</t>
+  </si>
+  <si>
+    <t>EndUserAccepted</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -719,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -742,17 +748,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB49C5B-9919-45C5-9892-FFA12CF07D74}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,9 +1066,10 @@
     <col min="5" max="5" width="31.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.109375" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>202</v>
       </c>
@@ -1072,8 +1091,11 @@
       <c r="G1" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>203</v>
       </c>
@@ -1090,7 +1112,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>203</v>
       </c>
@@ -1105,7 +1127,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>203</v>
       </c>
@@ -1122,7 +1144,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>203</v>
       </c>
@@ -1137,7 +1159,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>203</v>
       </c>
@@ -1151,8 +1173,11 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>203</v>
       </c>
@@ -1167,7 +1192,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>203</v>
       </c>
@@ -1184,7 +1209,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>203</v>
       </c>
@@ -1199,7 +1224,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>203</v>
       </c>
@@ -1213,8 +1238,11 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>203</v>
       </c>
@@ -1229,7 +1257,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>203</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>203</v>
       </c>
@@ -1260,8 +1288,11 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>203</v>
       </c>
@@ -1276,7 +1307,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>203</v>
       </c>
@@ -1293,7 +1324,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Optimized the performance by spliting the outputfile
</commit_message>
<xml_diff>
--- a/data/input/compare/mapping/Mapping.xlsx
+++ b/data/input/compare/mapping/Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Back-Ups\ExcelReportAnalyzer\xlreportanalyzer\data\input\compare\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B28BA2-93B7-484F-8FBD-53AFC1E05F19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39669360-AC88-4240-ABFB-6F3399322F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="1284" windowWidth="20364" windowHeight="11076" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB49C5B-9919-45C5-9892-FFA12CF07D74}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>